<commit_message>
Test cases by NFedan
</commit_message>
<xml_diff>
--- a/NFedan/TestCases.xlsx
+++ b/NFedan/TestCases.xlsx
@@ -318,7 +318,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -369,6 +369,15 @@
       <sz val="10"/>
       <color rgb="FF980000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="5">
@@ -424,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -541,6 +550,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
@@ -840,7 +852,9 @@
   </sheetPr>
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -854,7 +868,7 @@
     <col min="9" max="9" width="69.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.75">
+    <row r="1" spans="1:26" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -867,7 +881,7 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="42" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
@@ -7238,5 +7252,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>